<commit_message>
with 4 Scenarios Running
</commit_message>
<xml_diff>
--- a/KENTIM/DataSpreadsheets/LNG_Checks.xlsx
+++ b/KENTIM/DataSpreadsheets/LNG_Checks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\KENTIMGE\KENTIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1574AA99-D3B7-40D2-BCAE-7E1D9F5D8E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A356080-FFE9-4156-80D5-21A6B8111538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22FC1E87-AE5D-4C6B-9AFF-C347ADED527C}"/>
   </bookViews>
@@ -478,6 +478,50 @@
         <a:xfrm>
           <a:off x="13992225" y="4000500"/>
           <a:ext cx="6180952" cy="2085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>608686</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>84809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EADA1C2-2096-121C-A386-C0D8A196B783}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14420850" y="9525000"/>
+          <a:ext cx="7314286" cy="7323809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -788,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FBE569-75CB-4D55-937D-2F89F0151F57}">
   <dimension ref="B2:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,6 +1061,10 @@
         <v>5.2835648148148149</v>
       </c>
       <c r="E11" s="2"/>
+      <c r="H11">
+        <f>D11*T5*-PMT(0.08,30,1)</f>
+        <v>0.57419705842413293</v>
+      </c>
       <c r="L11" t="s">
         <v>19</v>
       </c>

</xml_diff>